<commit_message>
edit kolom tersembunyi akar permasalahan audit internal apotek
</commit_message>
<xml_diff>
--- a/audit/apotek/HASIL AUDIT INTENAL 1 PKM BERAKIT.xlsx
+++ b/audit/apotek/HASIL AUDIT INTENAL 1 PKM BERAKIT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7875"/>
+    <workbookView windowWidth="28800" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>HASIL TEMUAN AUDIT INTERNAL</t>
   </si>
@@ -55,7 +55,7 @@
     <t>Belum dilakukan konseling obat</t>
   </si>
   <si>
-    <t xml:space="preserve">SK Pendelegasian wewenang yang membantu apoteker di apotik tidak sesuai dengan pelaksanaan di lapangan </t>
+    <t>Belum terdapat fasilitas ruangan khusus konseling obat</t>
   </si>
   <si>
     <t>Lakukan konseling obat (2 bulan)</t>
@@ -70,6 +70,9 @@
     <t>Belum ada Prosedur pelaporan efek samping obat</t>
   </si>
   <si>
+    <t>Belum pernah ada pelaporan efek samping obat dari pasien</t>
+  </si>
+  <si>
     <t>Buat SOP Prosedur pelaporan efek samping obat (2 bulan)</t>
   </si>
   <si>
@@ -77,6 +80,9 @@
   </si>
   <si>
     <t>Belum tersedia box emergensi pada unit pelayanan</t>
+  </si>
+  <si>
+    <t>Obat emergensi selama ini belum ditempatkan pada box khusus</t>
   </si>
   <si>
     <t>Menyediakan box emergensi dan mengisi dengan BMHP yang dibutuhkan (2 bulan)</t>
@@ -87,12 +93,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,12 +132,110 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -140,32 +244,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -177,92 +260,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -277,192 +276,192 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -487,12 +486,64 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -518,6 +569,15 @@
         <color auto="1"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -526,15 +586,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -555,21 +606,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -599,11 +635,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -618,155 +660,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -780,19 +831,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1146,7 +1206,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6" outlineLevelCol="6"/>
@@ -1155,12 +1215,12 @@
     <col min="2" max="2" width="22.625" customWidth="1"/>
     <col min="3" max="3" width="43" customWidth="1"/>
     <col min="4" max="4" width="48.5666666666667" customWidth="1"/>
-    <col min="5" max="5" width="29.425" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="44.4166666666667" customWidth="1"/>
     <col min="6" max="6" width="50.2833333333333" customWidth="1"/>
     <col min="7" max="7" width="63.1416666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" ht="15" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1196,17 +1256,17 @@
       <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="12" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" ht="57" spans="1:7">
+    <row r="5" ht="42.75" spans="1:7">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -1216,52 +1276,56 @@
       <c r="C5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" ht="42.75" spans="1:7">
-      <c r="A6" s="4"/>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6" t="s">
+      <c r="E6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="F6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" ht="71.25" spans="1:7">
-      <c r="A7" s="4"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="6" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6" t="s">
+      <c r="D7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="E7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>